<commit_message>
add'l analysis for readme
</commit_message>
<xml_diff>
--- a/Data/mentorship_counts_compare.xlsx
+++ b/Data/mentorship_counts_compare.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8cfa97a60102b7d/Desktop/Analysis Projects/Pewlett-Hackard-Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F385DCC0-3DA1-455D-9022-7B129F4C8416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{F385DCC0-3DA1-455D-9022-7B129F4C8416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6270B9F-EAF1-4B47-9FF3-79BD28EAC9ED}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mentorship_counts_compare" sheetId="1" r:id="rId1"/>
+    <sheet name="compare by title" sheetId="2" r:id="rId1"/>
+    <sheet name="compare by dept" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Customer Service</t>
   </si>
@@ -61,24 +73,51 @@
     <t>% Of Total Active</t>
   </si>
   <si>
-    <t>Total Employees</t>
-  </si>
-  <si>
     <t>% Of Total Mentors</t>
   </si>
   <si>
     <t>Average Active Employees Per Mentor</t>
+  </si>
+  <si>
+    <t>Assistant Engineer</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Senior Engineer</t>
+  </si>
+  <si>
+    <t>Senior Staff</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Technique Leader</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Active and Mentorship Counts by Department</t>
+  </si>
+  <si>
+    <t>Active and Mentorship Counts by Title</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +252,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -395,7 +441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -510,6 +556,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -557,14 +612,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -922,11 +983,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AB9295-3D5A-4FDC-A5B7-547B1A595F0F}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,247 +999,492 @@
     <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:6" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>17569</v>
-      </c>
-      <c r="C2" s="3">
-        <f>ROUND(B2/$B$12,2)</f>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>120</v>
-      </c>
-      <c r="E2" s="3">
-        <f>ROUND(D2/$D$12,2)</f>
-        <v>0.08</v>
-      </c>
-      <c r="F2">
-        <f>ROUND(B2/D2,0)</f>
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>61386</v>
-      </c>
-      <c r="C3" s="3">
-        <f t="shared" ref="C3:C10" si="0">ROUND(B3/$B$12,2)</f>
-        <v>0.26</v>
-      </c>
-      <c r="D3" s="1">
-        <v>396</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E10" si="1">ROUND(D3/$D$12,2)</f>
-        <v>0.26</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F10" si="2">ROUND(B3/D3,0)</f>
-        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>12437</v>
+        <v>3588</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <f>ROUND(B4/$B$11,2)</f>
+        <v>0.01</v>
       </c>
       <c r="D4" s="1">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
+        <f>ROUND(D4/$D$11,2)</f>
+        <v>0.02</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
-        <v>194</v>
+        <f>ROUND(B4/D4,0)</f>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>12898</v>
+        <v>30983</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <f>ROUND(B5/$B$11,2)</f>
+        <v>0.13</v>
       </c>
       <c r="D5" s="1">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.06</v>
+        <f>ROUND(D5/$D$11,2)</f>
+        <v>0.12</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
-        <v>133</v>
+        <f>ROUND(B5/D5,0)</f>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
-        <v>14842</v>
+        <v>85939</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.06</v>
+        <f>ROUND(B6/$B$11,2)</f>
+        <v>0.36</v>
       </c>
       <c r="D6" s="1">
-        <v>117</v>
+        <v>529</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
+        <f>ROUND(D6/$D$11,2)</f>
+        <v>0.34</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
-        <v>127</v>
+        <f>ROUND(B6/D6,0)</f>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>53304</v>
+        <v>82024</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.22</v>
+        <f>ROUND(B7/$B$11,2)</f>
+        <v>0.34</v>
       </c>
       <c r="D7" s="1">
-        <v>322</v>
+        <v>569</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.21</v>
+        <f>ROUND(D7/$D$11,2)</f>
+        <v>0.37</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
-        <v>166</v>
+        <f>ROUND(B7/D7,0)</f>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1">
-        <v>14546</v>
+        <v>25526</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.06</v>
+        <f>ROUND(B8/$B$11,2)</f>
+        <v>0.11</v>
       </c>
       <c r="D8" s="1">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.06</v>
+        <f>ROUND(D8/$D$11,2)</f>
+        <v>0.1</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
-        <v>169</v>
+        <f>ROUND(B8/D8,0)</f>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>15441</v>
+        <v>12055</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
+        <f>ROUND(B9/$B$11,2)</f>
+        <v>0.05</v>
+      </c>
+      <c r="D9" s="1">
+        <v>77</v>
+      </c>
+      <c r="E9" s="3">
+        <f>ROUND(D9/$D$11,2)</f>
+        <v>0.05</v>
+      </c>
+      <c r="F9">
+        <f>ROUND(B9/D9,0)</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2">
+        <f>SUM(B1:B9)</f>
+        <v>240115</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2">
+        <f>SUM(D1:D9)</f>
+        <v>1549</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="6.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>17569</v>
+      </c>
+      <c r="C4" s="3">
+        <f>ROUND(B4/$B$14,2)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>120</v>
+      </c>
+      <c r="E4" s="3">
+        <f>ROUND(D4/$D$14,2)</f>
+        <v>0.08</v>
+      </c>
+      <c r="F4">
+        <f>ROUND(B4/D4,0)</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>61386</v>
+      </c>
+      <c r="C5" s="3">
+        <f>ROUND(B5/$B$14,2)</f>
+        <v>0.26</v>
+      </c>
+      <c r="D5" s="1">
+        <v>396</v>
+      </c>
+      <c r="E5" s="3">
+        <f>ROUND(D5/$D$14,2)</f>
+        <v>0.26</v>
+      </c>
+      <c r="F5">
+        <f>ROUND(B5/D5,0)</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12437</v>
+      </c>
+      <c r="C6" s="3">
+        <f>ROUND(B6/$B$14,2)</f>
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="1">
+        <v>64</v>
+      </c>
+      <c r="E6" s="3">
+        <f>ROUND(D6/$D$14,2)</f>
+        <v>0.04</v>
+      </c>
+      <c r="F6">
+        <f>ROUND(B6/D6,0)</f>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>12898</v>
+      </c>
+      <c r="C7" s="3">
+        <f>ROUND(B7/$B$14,2)</f>
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="1">
+        <v>97</v>
+      </c>
+      <c r="E7" s="3">
+        <f>ROUND(D7/$D$14,2)</f>
         <v>0.06</v>
       </c>
+      <c r="F7">
+        <f>ROUND(B7/D7,0)</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>14842</v>
+      </c>
+      <c r="C8" s="3">
+        <f>ROUND(B8/$B$14,2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D8" s="1">
+        <v>117</v>
+      </c>
+      <c r="E8" s="3">
+        <f>ROUND(D8/$D$14,2)</f>
+        <v>0.08</v>
+      </c>
+      <c r="F8">
+        <f>ROUND(B8/D8,0)</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>53304</v>
+      </c>
+      <c r="C9" s="3">
+        <f>ROUND(B9/$B$14,2)</f>
+        <v>0.22</v>
+      </c>
       <c r="D9" s="1">
-        <v>103</v>
+        <v>322</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(D9/$D$14,2)</f>
+        <v>0.21</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
-        <v>150</v>
+        <f>ROUND(B9/D9,0)</f>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>37701</v>
+        <v>14546</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>ROUND(B10/$B$14,2)</f>
+        <v>0.06</v>
       </c>
       <c r="D10" s="1">
-        <v>244</v>
+        <v>86</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="1"/>
-        <v>0.16</v>
+        <f>ROUND(D10/$D$14,2)</f>
+        <v>0.06</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>155</v>
+        <f>ROUND(B10/D10,0)</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>15441</v>
+      </c>
+      <c r="C11" s="3">
+        <f>ROUND(B11/$B$14,2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D11" s="1">
+        <v>103</v>
+      </c>
+      <c r="E11" s="3">
+        <f>ROUND(D11/$D$14,2)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F11">
+        <f>ROUND(B11/D11,0)</f>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2">
-        <f>SUM(B2:B10)</f>
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>37701</v>
+      </c>
+      <c r="C12" s="3">
+        <f>ROUND(B12/$B$14,2)</f>
+        <v>0.16</v>
+      </c>
+      <c r="D12" s="1">
+        <v>244</v>
+      </c>
+      <c r="E12" s="3">
+        <f>ROUND(D12/$D$14,2)</f>
+        <v>0.16</v>
+      </c>
+      <c r="F12">
+        <f>ROUND(B12/D12,0)</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <f>SUM(B4:B12)</f>
         <v>240124</v>
       </c>
-      <c r="D12" s="2">
-        <f>SUM(D2:D10)</f>
+      <c r="D14" s="2">
+        <f>SUM(D4:D12)</f>
         <v>1549</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>